<commit_message>
Actualizaciones de planillas Modificación encabezado de edición de lances
</commit_message>
<xml_diff>
--- a/Curso/Planillas con datos/DatosLances.xlsx
+++ b/Curso/Planillas con datos/DatosLances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="152">
   <si>
     <t>nro_boya</t>
   </si>
@@ -222,18 +222,12 @@
     <t>63° 55,87´</t>
   </si>
   <si>
-    <t>45° 55,62´</t>
-  </si>
-  <si>
     <t>63° 55,91´</t>
   </si>
   <si>
     <t>63° 56,75´</t>
   </si>
   <si>
-    <t>45° 55,72´</t>
-  </si>
-  <si>
     <t>63° 57,89´</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>63° 58,02´</t>
   </si>
   <si>
-    <t>45° 57,87´</t>
-  </si>
-  <si>
     <t>63° 59,10´</t>
   </si>
   <si>
@@ -264,18 +255,12 @@
     <t>63° 59,06´</t>
   </si>
   <si>
-    <t>45° 59,08´</t>
-  </si>
-  <si>
     <t>63° 59,33´</t>
   </si>
   <si>
     <t>63° 59,41´</t>
   </si>
   <si>
-    <t>45° 59,47´</t>
-  </si>
-  <si>
     <t>63° 59,48´</t>
   </si>
   <si>
@@ -285,27 +270,18 @@
     <t>63° 59,54´</t>
   </si>
   <si>
-    <t>45° 59,58´</t>
-  </si>
-  <si>
     <t>64° 03,37´</t>
   </si>
   <si>
     <t>64° 03,45´</t>
   </si>
   <si>
-    <t>45° 03,45´</t>
-  </si>
-  <si>
     <t>64° 03,52´</t>
   </si>
   <si>
     <t>64° 03,60´</t>
   </si>
   <si>
-    <t>45° 03,68´</t>
-  </si>
-  <si>
     <t>64° 03,54´</t>
   </si>
   <si>
@@ -315,9 +291,6 @@
     <t>64° 03,35´</t>
   </si>
   <si>
-    <t>45° 03,77´</t>
-  </si>
-  <si>
     <t>distancia_entre_trampas</t>
   </si>
   <si>
@@ -475,6 +448,30 @@
   </si>
   <si>
     <t>16/11/2014</t>
+  </si>
+  <si>
+    <t>63° 55,62´</t>
+  </si>
+  <si>
+    <t>63° 55,72´</t>
+  </si>
+  <si>
+    <t>63° 57,87´</t>
+  </si>
+  <si>
+    <t>63° 59,08´</t>
+  </si>
+  <si>
+    <t>63° 59,47´</t>
+  </si>
+  <si>
+    <t>63° 59,58´</t>
+  </si>
+  <si>
+    <t>64° 03,77´</t>
+  </si>
+  <si>
+    <t>64° 03,68´</t>
   </si>
 </sst>
 </file>
@@ -819,7 +816,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +829,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -844,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -925,7 +922,7 @@
         <v>64</v>
       </c>
       <c r="AF1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -960,16 +957,16 @@
         <v>24</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P2">
         <v>91</v>
@@ -990,16 +987,16 @@
         <v>66</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Z2">
         <v>91</v>
@@ -1017,10 +1014,10 @@
         <v>28</v>
       </c>
       <c r="AE2" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="AF2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -1055,16 +1052,16 @@
         <v>24</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="P3">
         <v>94</v>
@@ -1082,19 +1079,19 @@
         <v>30</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="Z3">
         <v>94</v>
@@ -1106,13 +1103,13 @@
         <v>31</v>
       </c>
       <c r="AC3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD3" t="s">
         <v>32</v>
       </c>
       <c r="AE3" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -1147,16 +1144,16 @@
         <v>24</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="P4">
         <v>94</v>
@@ -1168,25 +1165,25 @@
         <v>30</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="Z4">
         <v>86</v>
@@ -1198,13 +1195,13 @@
         <v>34</v>
       </c>
       <c r="AC4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AD4" t="s">
         <v>30</v>
       </c>
       <c r="AE4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1242,16 +1239,16 @@
         <v>24</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="P5">
         <v>85</v>
@@ -1263,25 +1260,25 @@
         <v>35</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="Z5">
         <v>81</v>
@@ -1293,16 +1290,16 @@
         <v>37</v>
       </c>
       <c r="AC5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD5" t="s">
         <v>38</v>
       </c>
       <c r="AE5" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="AF5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -1337,16 +1334,16 @@
         <v>24</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="P6">
         <v>93</v>
@@ -1358,25 +1355,25 @@
         <v>39</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="T6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="Z6">
         <v>93</v>
@@ -1388,13 +1385,13 @@
         <v>41</v>
       </c>
       <c r="AC6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AD6" t="s">
         <v>42</v>
       </c>
       <c r="AE6" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1420,16 +1417,16 @@
         <v>24</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="P7">
         <v>93</v>
@@ -1441,25 +1438,25 @@
         <v>43</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="Z7">
         <v>93</v>
@@ -1471,16 +1468,16 @@
         <v>43</v>
       </c>
       <c r="AC7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AD7" t="s">
         <v>44</v>
       </c>
       <c r="AE7" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="AF7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -1515,16 +1512,16 @@
         <v>24</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="P8">
         <v>93</v>
@@ -1536,25 +1533,25 @@
         <v>45</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="Z8">
         <v>94</v>
@@ -1566,13 +1563,13 @@
         <v>47</v>
       </c>
       <c r="AC8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AD8" t="s">
         <v>48</v>
       </c>
       <c r="AE8" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -1607,16 +1604,16 @@
         <v>55</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="P9">
         <v>96</v>
@@ -1628,40 +1625,40 @@
         <v>56</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="T9" s="2" t="s">
         <v>57</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="AB9" t="s">
         <v>58</v>
       </c>
       <c r="AC9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="AD9" t="s">
         <v>59</v>
       </c>
       <c r="AE9" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="AF9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -1690,16 +1687,16 @@
         <v>24</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P10">
         <v>95</v>
@@ -1711,25 +1708,25 @@
         <v>49</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="Z10">
         <v>95</v>
@@ -1741,16 +1738,16 @@
         <v>49</v>
       </c>
       <c r="AC10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="AD10" t="s">
         <v>50</v>
       </c>
       <c r="AE10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="AF10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -1785,16 +1782,16 @@
         <v>24</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="P11">
         <v>95</v>
@@ -1806,25 +1803,25 @@
         <v>51</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="Z11">
         <v>95</v>
@@ -1836,16 +1833,16 @@
         <v>53</v>
       </c>
       <c r="AC11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="AD11" t="s">
         <v>54</v>
       </c>
       <c r="AE11" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="AF11" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>